<commit_message>
code cleaning and update new cahnges
</commit_message>
<xml_diff>
--- a/Data Transfer Template.xlsx
+++ b/Data Transfer Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\New folder (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EFAAB9-FD9E-4B6B-9AB9-0EF535F8F1B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1BC2DF-F12E-4469-86BF-3FA9EB84EE3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{B086B3B7-105E-4E8F-B634-8F687F959483}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>Host</t>
   </si>
   <si>
-    <t>34.171.176.139</t>
-  </si>
-  <si>
     <t>Hostname of source DW</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>claim</t>
+  </si>
+  <si>
+    <t>34.31.79.171</t>
   </si>
 </sst>
 </file>
@@ -676,38 +676,38 @@
   <sheetData>
     <row r="1" spans="1:3" ht="390" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -774,7 +774,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -888,76 +888,76 @@
         <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
         <v>1025</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -984,37 +984,37 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2"/>
     </row>

</xml_diff>